<commit_message>
Added Chat Bot Crud API's
</commit_message>
<xml_diff>
--- a/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
+++ b/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opo119738\Desktop\Project Details\BotHub\Git_API\APIs\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opo119738\Desktop\Project Details\BotHub\Git_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1341,13 +1341,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.69921875" defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="150">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="41.4">
+    <row r="4" spans="1:6" ht="27.6">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="210">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="240">
+    <row r="8" spans="1:6" ht="75">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="141.6">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="225">
+    <row r="13" spans="1:6" ht="45">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="135">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="41.4">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="390">
+    <row r="17" spans="1:6" ht="409.6">
       <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="195">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="27.6">
+    <row r="21" spans="1:6" ht="15">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="41.4">
+    <row r="22" spans="1:6" ht="15">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="207">
+    <row r="28" spans="1:6" ht="69">
       <c r="A28" s="2" t="s">
         <v>91</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="289.8">
+    <row r="30" spans="1:6" ht="82.8">
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="165.6">
+    <row r="31" spans="1:6" ht="151.80000000000001">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Added Call Broadcast API and get Recorded audio files in Auth application for voice bot
</commit_message>
<xml_diff>
--- a/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
+++ b/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="129">
   <si>
     <t>API Name</t>
   </si>
@@ -927,6 +927,57 @@
         {"from_node": 1, "to_node": 2, "edge_type": "direct"}
     ]
 }</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/call/Broadcast/</t>
+  </si>
+  <si>
+    <t>{
+    "agent_id": 1,
+    "user_id":1,
+    "group_id":1,
+    "phone_numbers": [
+      { 
+          "name": "naga", "number": "9821209237","contact_id":"1" 
+           }
+     ]
+  }</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/call/Broadcast/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "agent_id": 1,
+    "user_id":1,
+    "group_id":1,
+    "phone_numbers": [
+      { 
+          "name": "naga", "number": "9821209237","contact_id":"1" 
+           }
+     ]
+  }
+ '</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/get/recorded/audio/file/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get Recorded audio file     ( POST ) </t>
+  </si>
+  <si>
+    <t>Call Broadcast   ( POST )</t>
+  </si>
+  <si>
+    <t>{
+    "file_path": "/usr/share/freeswitch/var/lib/freeswitch/recordings/c6b69a41-dec9-4257-b061-50b3da35b3e6.wav"
+}</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/get/recorded/audio/file/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "file_path": "/usr/share/freeswitch/var/lib/freeswitch/recordings/c6b69a41-dec9-4257-b061-50b3da35b3e6.wav"
+}'</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1004,6 +1055,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1339,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.69921875" defaultRowHeight="13.8"/>
@@ -1923,12 +1975,42 @@
         <v>111</v>
       </c>
     </row>
+    <row r="36" spans="1:5" ht="248.4">
+      <c r="A36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="110.4">
+      <c r="A39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C17" r:id="rId2" display="http://1msg.1point1.in:3001/api/auth/j-v1/call-history/by-number/?number=123456&amp;user_id=1"/>
+    <hyperlink ref="B36" r:id="rId3"/>
+    <hyperlink ref="B39" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Voice Bot get Conversation History
</commit_message>
<xml_diff>
--- a/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
+++ b/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
   <si>
     <t>API Name</t>
   </si>
@@ -996,6 +996,30 @@
   </si>
   <si>
     <t>get call transcription</t>
+  </si>
+  <si>
+    <t>get conversation history ( POST )</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/get/conversation/history/</t>
+  </si>
+  <si>
+    <t>{
+    "user_id" : 11,
+    "agent_id": 72 ,
+    "from_date" : "2025-05-18" ,
+    "to_date" : "2025-05-18"
+}</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/get/conversation/history/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "user_id" : 11,
+    "agent_id": 72 ,
+    "from_date" : "2025-05-18" ,
+    "to_date" : "2025-05-18"
+}'</t>
   </si>
 </sst>
 </file>
@@ -1409,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.69921875" defaultRowHeight="13.8"/>
@@ -2035,6 +2059,20 @@
         <v>131</v>
       </c>
     </row>
+    <row r="45" spans="1:5" ht="124.2">
+      <c r="A45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -2042,8 +2080,9 @@
     <hyperlink ref="B36" r:id="rId3"/>
     <hyperlink ref="B39" r:id="rId4"/>
     <hyperlink ref="B42" r:id="rId5"/>
+    <hyperlink ref="B45" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added update agent status API for ALl the bots
</commit_message>
<xml_diff>
--- a/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
+++ b/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="141">
   <si>
     <t>API Name</t>
   </si>
@@ -1020,6 +1020,30 @@
     "from_date" : "2025-05-18" ,
     "to_date" : "2025-05-18"
 }'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Voice Bot  Agent Status ( PUT )
+</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/update/agent/status/</t>
+  </si>
+  <si>
+    <t>{
+    "user_id" : 10,
+    "agent_id" : 78,
+    "agent_status" : true
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">curl --location --request PUT 'http://1msg.1point1.in:3001/api/auth/j-v1/update/agent/status/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "user_id" : 10,
+    "agent_id" : 78,
+    "agent_status" : true
+}'
+</t>
   </si>
 </sst>
 </file>
@@ -1433,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.69921875" defaultRowHeight="13.8"/>
@@ -2071,6 +2095,20 @@
       </c>
       <c r="D45" s="6" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="151.80000000000001">
+      <c r="A48" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Voice bot report API
</commit_message>
<xml_diff>
--- a/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
+++ b/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="145">
   <si>
     <t>API Name</t>
   </si>
@@ -142,6 +142,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
       </rPr>
       <t>name</t>
     </r>
@@ -160,6 +161,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
       </rPr>
       <t>phonenumber</t>
     </r>
@@ -1045,6 +1047,28 @@
 }'
 </t>
   </si>
+  <si>
+    <t>Voice Bot Report   ( POST )</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/report/voicebot/agent_id/</t>
+  </si>
+  <si>
+    <t>{
+  "agent_id": 1,
+  "from_date": "2025-01-01",
+  "to_date": "2025-12-31"
+}</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/report/voicebot/agent_id/' \
+--header 'Content-Type: application/json' \
+--data '{
+  "agent_id": 1,
+  "from_date": "2025-01-01",
+  "to_date": "2025-12-31"
+}'</t>
+  </si>
 </sst>
 </file>
 
@@ -1070,6 +1094,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1101,7 +1126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1122,6 +1147,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1457,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.69921875" defaultRowHeight="13.8"/>
@@ -2109,6 +2137,20 @@
       </c>
       <c r="D48" s="6" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="110.4">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2119,8 +2161,9 @@
     <hyperlink ref="B39" r:id="rId4"/>
     <hyperlink ref="B42" r:id="rId5"/>
     <hyperlink ref="B45" r:id="rId6"/>
+    <hyperlink ref="B51" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2 API Get Call History by user and Get Uniq Dispositions
</commit_message>
<xml_diff>
--- a/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
+++ b/Authentication_&_Voice_Bot_APIs_by_Puru.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="160">
   <si>
     <t>API Name</t>
   </si>
@@ -1106,6 +1106,39 @@
   "from_date": "2025-01-01",
   "to_date": "2025-12-31"
 }'</t>
+  </si>
+  <si>
+    <t>Dashboard Voice Bot ( GET )</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/dashboard/voice/bot/?user_id=6</t>
+  </si>
+  <si>
+    <t>user_id=6</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/dashboard/voice/bot/?user_id=6'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Call History by Agent ID    ( GET )   </t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/call-history/by/user_id/?user_id=1</t>
+  </si>
+  <si>
+    <t>user_id=10</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/call-history/by/user_id/?user_id=10'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Unique Dispositions ( GET )  </t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/auth/j-v1/get/unique-disposition/</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/auth/j-v1/get/unique-disposition/'</t>
   </si>
 </sst>
 </file>
@@ -1523,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.69921875" defaultRowHeight="13.8"/>
@@ -2203,6 +2236,45 @@
       </c>
       <c r="D54" s="6" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2215,8 +2287,11 @@
     <hyperlink ref="B45" r:id="rId6"/>
     <hyperlink ref="B51" r:id="rId7"/>
     <hyperlink ref="B54" r:id="rId8"/>
+    <hyperlink ref="B57" r:id="rId9"/>
+    <hyperlink ref="B60" r:id="rId10"/>
+    <hyperlink ref="B63" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>